<commit_message>
DSE_FH_ScAg_002:Add input and specific requirements
</commit_message>
<xml_diff>
--- a/1) Requirements/SWRA_20190405.xlsx
+++ b/1) Requirements/SWRA_20190405.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="89">
   <si>
     <t>No.</t>
   </si>
@@ -214,20 +214,198 @@
     <t xml:space="preserve">Power Circuit Control </t>
   </si>
   <si>
-    <t xml:space="preserve">Motor Connections Electrical B7Diagram </t>
-  </si>
-  <si>
     <t>Hardware Version</t>
   </si>
   <si>
     <t>6- Verifiable.</t>
+  </si>
+  <si>
+    <t>RQ-SYS.007</t>
+  </si>
+  <si>
+    <t>PWM voltage shall be at 13.5V</t>
+  </si>
+  <si>
+    <t>RQ-SYS.008</t>
+  </si>
+  <si>
+    <t>Frequency rate shall be 10Khz</t>
+  </si>
+  <si>
+    <t>RQ-SYS.009</t>
+  </si>
+  <si>
+    <t>Max Duty cycle percentage shall be 100%</t>
+  </si>
+  <si>
+    <t>RQ-SYS.010</t>
+  </si>
+  <si>
+    <t>Minimum duty cycle percentage shall be 0%</t>
+  </si>
+  <si>
+    <t>RQ-SYS.011</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RPMs shall be similar as is described at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sección 1.2.2.1 Tabla 1: Valores sin carga del motors @13.6V </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">in the document </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>20190501c Requisitos del proyecto Integrador CESEQ.docx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>RQ-SYS.012</t>
+  </si>
+  <si>
+    <t>RQ-SYS.013</t>
+  </si>
+  <si>
+    <t>Set point shall be set by using UART communications and defining its own communication protocol</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set point shall be using is a potentiometer as is described at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sección 1.2.2.1 Figura 5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">in the document </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>20190501c Requisitos del proyecto Integrador CESEQ.docx</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor Connections Electrical Diagram </t>
+  </si>
+  <si>
+    <t>RQ-SYS.016</t>
+  </si>
+  <si>
+    <t>RQ-SYS.017</t>
+  </si>
+  <si>
+    <t>RQ-SYS.014</t>
+  </si>
+  <si>
+    <t>RQ-SYS.014.1</t>
+  </si>
+  <si>
+    <t>RQ-SYS.015</t>
+  </si>
+  <si>
+    <t>Integrate Circuit DRV8848-2A shall be use as H-Bridge</t>
+  </si>
+  <si>
+    <t>Motor shall has with a diode as free or reverse spin</t>
+  </si>
+  <si>
+    <t>Motor shall has with source power for hall-effect sensor</t>
+  </si>
+  <si>
+    <t>Motor shall has with an designed ouput for the hall-effect sensor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El diagrama se encuentra en la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Seccion 1.3.2.2 Figura7 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">del documento </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>20190501c Requisitos 
+del proyecto Integrador CESEQ.docx</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +488,14 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,7 +607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -520,6 +706,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -792,7 +1015,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -800,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N131"/>
+  <dimension ref="A1:N130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +1070,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>7</v>
@@ -1627,7 +1850,7 @@
         <v>47</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>16</v>
@@ -1797,119 +2020,317 @@
       <c r="N27" s="29"/>
     </row>
     <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
+      <c r="A28" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28" s="38" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
+      <c r="A29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29" s="38" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
+      <c r="A30" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="38" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-    </row>
-    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-    </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
+      <c r="A31" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31" s="38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32" s="38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N33" s="38" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="29"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
+      <c r="A34" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="L34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="M34" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="N34" s="39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A35" s="43" t="s">
+        <v>81</v>
+      </c>
       <c r="B35" s="6"/>
       <c r="C35" s="26"/>
       <c r="D35" s="29"/>
@@ -1963,7 +2384,7 @@
     <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
       <c r="B38" s="8" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C38" s="27"/>
       <c r="D38" s="30"/>
@@ -1978,105 +2399,245 @@
       <c r="M38" s="30"/>
       <c r="N38" s="30"/>
     </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="29"/>
-    </row>
-    <row r="40" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
+    <row r="39" spans="1:14" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A39" s="41"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="45"/>
+    </row>
+    <row r="40" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="L40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="M40" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40" s="46" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
-      <c r="N41" s="29"/>
+      <c r="A41" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="L41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="46" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
+      <c r="A42" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="L42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="46" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
+      <c r="A43" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="L43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="M43" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="N43" s="46" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-    </row>
-    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="15"/>
+      <c r="A44" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="L44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="M44" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="N44" s="46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="6"/>
       <c r="C45" s="26"/>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -2090,39 +2651,39 @@
       <c r="M45" s="29"/>
       <c r="N45" s="29"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
-      <c r="N46" s="29"/>
+    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A46" s="11"/>
+      <c r="B46" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="27"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="30"/>
     </row>
     <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A47" s="11"/>
-      <c r="B47" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
     </row>
     <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
@@ -2140,9 +2701,9 @@
       <c r="M48" s="29"/>
       <c r="N48" s="29"/>
     </row>
-    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="15"/>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="10"/>
+      <c r="B49" s="6"/>
       <c r="C49" s="26"/>
       <c r="D49" s="29"/>
       <c r="E49" s="29"/>
@@ -2156,39 +2717,39 @@
       <c r="M49" s="29"/>
       <c r="N49" s="29"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
+    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A50" s="11"/>
+      <c r="B50" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="27"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="30"/>
+      <c r="M50" s="30"/>
+      <c r="N50" s="30"/>
     </row>
     <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A51" s="11"/>
-      <c r="B51" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="27"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
     </row>
     <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
@@ -2207,74 +2768,74 @@
       <c r="N52" s="29"/>
     </row>
     <row r="53" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="5"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="15"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
-      <c r="N53" s="29"/>
-    </row>
-    <row r="54" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A54" s="16"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="18"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
-      <c r="N55" s="29"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="12"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="29"/>
+      <c r="M54" s="29"/>
+      <c r="N54" s="29"/>
+    </row>
+    <row r="55" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A55" s="11"/>
+      <c r="B55" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="30"/>
+      <c r="L55" s="30"/>
+      <c r="M55" s="30"/>
+      <c r="N55" s="30"/>
     </row>
     <row r="56" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="11"/>
-      <c r="B56" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="30"/>
-      <c r="K56" s="30"/>
-      <c r="L56" s="30"/>
-      <c r="M56" s="30"/>
-      <c r="N56" s="30"/>
-    </row>
-    <row r="57" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" s="13"/>
-      <c r="B57" s="15"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
+      <c r="K56" s="29"/>
+      <c r="L56" s="29"/>
+      <c r="M56" s="29"/>
+      <c r="N56" s="29"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" s="10"/>
+      <c r="B57" s="6"/>
       <c r="C57" s="26"/>
       <c r="D57" s="29"/>
       <c r="E57" s="29"/>
@@ -2288,43 +2849,43 @@
       <c r="M57" s="29"/>
       <c r="N57" s="29"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="29"/>
-      <c r="N58" s="29"/>
+    <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A58" s="11"/>
+      <c r="B58" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" s="27"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="30"/>
+      <c r="J58" s="30"/>
+      <c r="K58" s="30"/>
+      <c r="L58" s="30"/>
+      <c r="M58" s="30"/>
+      <c r="N58" s="30"/>
     </row>
     <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" s="11"/>
-      <c r="B59" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="30"/>
-      <c r="I59" s="30"/>
-      <c r="J59" s="30"/>
-      <c r="K59" s="30"/>
-      <c r="L59" s="30"/>
-      <c r="M59" s="30"/>
-      <c r="N59" s="30"/>
-    </row>
-    <row r="60" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A60" s="13"/>
-      <c r="B60" s="15"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
+      <c r="J59" s="29"/>
+      <c r="K59" s="29"/>
+      <c r="L59" s="29"/>
+      <c r="M59" s="29"/>
+      <c r="N59" s="29"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" s="19"/>
+      <c r="B60" s="6"/>
       <c r="C60" s="26"/>
       <c r="D60" s="29"/>
       <c r="E60" s="29"/>
@@ -2435,7 +2996,7 @@
       <c r="N66" s="29"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A67" s="19"/>
+      <c r="A67" s="12"/>
       <c r="B67" s="6"/>
       <c r="C67" s="26"/>
       <c r="D67" s="29"/>
@@ -2450,43 +3011,43 @@
       <c r="M67" s="29"/>
       <c r="N67" s="29"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A68" s="12"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
-      <c r="K68" s="29"/>
-      <c r="L68" s="29"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="29"/>
+    <row r="68" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A68" s="11"/>
+      <c r="B68" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68" s="27"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="30"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="30"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="30"/>
+      <c r="N68" s="30"/>
     </row>
     <row r="69" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A69" s="11"/>
-      <c r="B69" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C69" s="27"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="30"/>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30"/>
-      <c r="K69" s="30"/>
-      <c r="L69" s="30"/>
-      <c r="M69" s="30"/>
-      <c r="N69" s="30"/>
-    </row>
-    <row r="70" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A70" s="14"/>
-      <c r="B70" s="15"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="29"/>
+      <c r="K69" s="29"/>
+      <c r="L69" s="29"/>
+      <c r="M69" s="29"/>
+      <c r="N69" s="29"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A70" s="20"/>
+      <c r="B70" s="6"/>
       <c r="C70" s="26"/>
       <c r="D70" s="29"/>
       <c r="E70" s="29"/>
@@ -2501,7 +3062,7 @@
       <c r="N70" s="29"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A71" s="20"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="6"/>
       <c r="C71" s="26"/>
       <c r="D71" s="29"/>
@@ -2533,7 +3094,7 @@
       <c r="N72" s="29"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A73" s="19"/>
+      <c r="A73" s="20"/>
       <c r="B73" s="6"/>
       <c r="C73" s="26"/>
       <c r="D73" s="29"/>
@@ -2549,7 +3110,7 @@
       <c r="N73" s="29"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A74" s="20"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="6"/>
       <c r="C74" s="26"/>
       <c r="D74" s="29"/>
@@ -2581,7 +3142,7 @@
       <c r="N75" s="29"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A76" s="19"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="6"/>
       <c r="C76" s="26"/>
       <c r="D76" s="29"/>
@@ -2597,7 +3158,7 @@
       <c r="N76" s="29"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A77" s="20"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="6"/>
       <c r="C77" s="26"/>
       <c r="D77" s="29"/>
@@ -2613,7 +3174,7 @@
       <c r="N77" s="29"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A78" s="19"/>
+      <c r="A78" s="12"/>
       <c r="B78" s="6"/>
       <c r="C78" s="26"/>
       <c r="D78" s="29"/>
@@ -2628,42 +3189,42 @@
       <c r="M78" s="29"/>
       <c r="N78" s="29"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A79" s="12"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
-      <c r="G79" s="29"/>
-      <c r="H79" s="29"/>
-      <c r="I79" s="29"/>
-      <c r="J79" s="29"/>
-      <c r="K79" s="29"/>
-      <c r="L79" s="29"/>
-      <c r="M79" s="29"/>
-      <c r="N79" s="29"/>
+    <row r="79" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A79" s="11"/>
+      <c r="B79" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79" s="27"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="30"/>
+      <c r="G79" s="30"/>
+      <c r="H79" s="30"/>
+      <c r="I79" s="30"/>
+      <c r="J79" s="30"/>
+      <c r="K79" s="30"/>
+      <c r="L79" s="30"/>
+      <c r="M79" s="30"/>
+      <c r="N79" s="30"/>
     </row>
     <row r="80" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A80" s="11"/>
-      <c r="B80" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C80" s="27"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="30"/>
-      <c r="G80" s="30"/>
-      <c r="H80" s="30"/>
-      <c r="I80" s="30"/>
-      <c r="J80" s="30"/>
-      <c r="K80" s="30"/>
-      <c r="L80" s="30"/>
-      <c r="M80" s="30"/>
-      <c r="N80" s="30"/>
+      <c r="A80" s="23"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="29"/>
+      <c r="K80" s="29"/>
+      <c r="L80" s="29"/>
+      <c r="M80" s="29"/>
+      <c r="N80" s="29"/>
     </row>
     <row r="81" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A81" s="23"/>
+      <c r="A81" s="13"/>
       <c r="B81" s="15"/>
       <c r="C81" s="26"/>
       <c r="D81" s="29"/>
@@ -2792,7 +3353,7 @@
     </row>
     <row r="89" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
-      <c r="B89" s="15"/>
+      <c r="B89" s="6"/>
       <c r="C89" s="26"/>
       <c r="D89" s="29"/>
       <c r="E89" s="29"/>
@@ -2823,41 +3384,41 @@
       <c r="N90" s="29"/>
     </row>
     <row r="91" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A91" s="13"/>
-      <c r="B91" s="6"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="29"/>
-      <c r="E91" s="29"/>
-      <c r="F91" s="29"/>
-      <c r="G91" s="29"/>
-      <c r="H91" s="29"/>
-      <c r="I91" s="29"/>
-      <c r="J91" s="29"/>
-      <c r="K91" s="29"/>
-      <c r="L91" s="29"/>
-      <c r="M91" s="29"/>
-      <c r="N91" s="29"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C91" s="27"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="30"/>
+      <c r="G91" s="30"/>
+      <c r="H91" s="30"/>
+      <c r="I91" s="30"/>
+      <c r="J91" s="30"/>
+      <c r="K91" s="30"/>
+      <c r="L91" s="30"/>
+      <c r="M91" s="30"/>
+      <c r="N91" s="30"/>
     </row>
     <row r="92" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A92" s="11"/>
-      <c r="B92" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C92" s="27"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="30"/>
-      <c r="G92" s="30"/>
-      <c r="H92" s="30"/>
-      <c r="I92" s="30"/>
-      <c r="J92" s="30"/>
-      <c r="K92" s="30"/>
-      <c r="L92" s="30"/>
-      <c r="M92" s="30"/>
-      <c r="N92" s="30"/>
+      <c r="A92" s="22"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="29"/>
+      <c r="J92" s="29"/>
+      <c r="K92" s="29"/>
+      <c r="L92" s="29"/>
+      <c r="M92" s="29"/>
+      <c r="N92" s="29"/>
     </row>
     <row r="93" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A93" s="22"/>
+      <c r="A93" s="13"/>
       <c r="B93" s="15"/>
       <c r="C93" s="26"/>
       <c r="D93" s="29"/>
@@ -2872,8 +3433,8 @@
       <c r="M93" s="29"/>
       <c r="N93" s="29"/>
     </row>
-    <row r="94" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A94" s="13"/>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A94" s="21"/>
       <c r="B94" s="15"/>
       <c r="C94" s="26"/>
       <c r="D94" s="29"/>
@@ -2936,8 +3497,8 @@
       <c r="M97" s="29"/>
       <c r="N97" s="29"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A98" s="21"/>
+    <row r="98" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A98" s="13"/>
       <c r="B98" s="15"/>
       <c r="C98" s="26"/>
       <c r="D98" s="29"/>
@@ -3016,9 +3577,9 @@
       <c r="M102" s="29"/>
       <c r="N102" s="29"/>
     </row>
-    <row r="103" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A103" s="13"/>
-      <c r="B103" s="15"/>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A103" s="12"/>
+      <c r="B103" s="6"/>
       <c r="C103" s="26"/>
       <c r="D103" s="29"/>
       <c r="E103" s="29"/>
@@ -3032,41 +3593,41 @@
       <c r="M103" s="29"/>
       <c r="N103" s="29"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A104" s="12"/>
-      <c r="B104" s="6"/>
-      <c r="C104" s="26"/>
-      <c r="D104" s="29"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="29"/>
-      <c r="G104" s="29"/>
-      <c r="H104" s="29"/>
-      <c r="I104" s="29"/>
-      <c r="J104" s="29"/>
-      <c r="K104" s="29"/>
-      <c r="L104" s="29"/>
-      <c r="M104" s="29"/>
-      <c r="N104" s="29"/>
+    <row r="104" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A104" s="11"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="30"/>
+      <c r="E104" s="30"/>
+      <c r="F104" s="30"/>
+      <c r="G104" s="30"/>
+      <c r="H104" s="30"/>
+      <c r="I104" s="30"/>
+      <c r="J104" s="30"/>
+      <c r="K104" s="30"/>
+      <c r="L104" s="30"/>
+      <c r="M104" s="30"/>
+      <c r="N104" s="30"/>
     </row>
     <row r="105" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A105" s="11"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="27"/>
-      <c r="D105" s="30"/>
-      <c r="E105" s="30"/>
-      <c r="F105" s="30"/>
-      <c r="G105" s="30"/>
-      <c r="H105" s="30"/>
-      <c r="I105" s="30"/>
-      <c r="J105" s="30"/>
-      <c r="K105" s="30"/>
-      <c r="L105" s="30"/>
-      <c r="M105" s="30"/>
-      <c r="N105" s="30"/>
-    </row>
-    <row r="106" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A106" s="13"/>
-      <c r="B106" s="15"/>
+      <c r="A105" s="13"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="26"/>
+      <c r="D105" s="29"/>
+      <c r="E105" s="29"/>
+      <c r="F105" s="29"/>
+      <c r="G105" s="29"/>
+      <c r="H105" s="29"/>
+      <c r="I105" s="29"/>
+      <c r="J105" s="29"/>
+      <c r="K105" s="29"/>
+      <c r="L105" s="29"/>
+      <c r="M105" s="29"/>
+      <c r="N105" s="29"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A106" s="10"/>
+      <c r="B106" s="6"/>
       <c r="C106" s="26"/>
       <c r="D106" s="29"/>
       <c r="E106" s="29"/>
@@ -3080,40 +3641,40 @@
       <c r="M106" s="29"/>
       <c r="N106" s="29"/>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A107" s="10"/>
-      <c r="B107" s="6"/>
-      <c r="C107" s="26"/>
-      <c r="D107" s="29"/>
-      <c r="E107" s="29"/>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="29"/>
-      <c r="I107" s="29"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="29"/>
-      <c r="L107" s="29"/>
-      <c r="M107" s="29"/>
-      <c r="N107" s="29"/>
+    <row r="107" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A107" s="11"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="30"/>
+      <c r="E107" s="30"/>
+      <c r="F107" s="30"/>
+      <c r="G107" s="30"/>
+      <c r="H107" s="30"/>
+      <c r="I107" s="30"/>
+      <c r="J107" s="30"/>
+      <c r="K107" s="30"/>
+      <c r="L107" s="30"/>
+      <c r="M107" s="30"/>
+      <c r="N107" s="30"/>
     </row>
     <row r="108" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A108" s="11"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="30"/>
-      <c r="E108" s="30"/>
-      <c r="F108" s="30"/>
-      <c r="G108" s="30"/>
-      <c r="H108" s="30"/>
-      <c r="I108" s="30"/>
-      <c r="J108" s="30"/>
-      <c r="K108" s="30"/>
-      <c r="L108" s="30"/>
-      <c r="M108" s="30"/>
-      <c r="N108" s="30"/>
+      <c r="A108" s="22"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="26"/>
+      <c r="D108" s="29"/>
+      <c r="E108" s="29"/>
+      <c r="F108" s="29"/>
+      <c r="G108" s="29"/>
+      <c r="H108" s="29"/>
+      <c r="I108" s="29"/>
+      <c r="J108" s="29"/>
+      <c r="K108" s="29"/>
+      <c r="L108" s="29"/>
+      <c r="M108" s="29"/>
+      <c r="N108" s="29"/>
     </row>
     <row r="109" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A109" s="22"/>
+      <c r="A109" s="13"/>
       <c r="B109" s="15"/>
       <c r="C109" s="26"/>
       <c r="D109" s="29"/>
@@ -3208,9 +3769,9 @@
       <c r="M114" s="29"/>
       <c r="N114" s="29"/>
     </row>
-    <row r="115" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A115" s="13"/>
-      <c r="B115" s="15"/>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A115" s="12"/>
+      <c r="B115" s="6"/>
       <c r="C115" s="26"/>
       <c r="D115" s="29"/>
       <c r="E115" s="29"/>
@@ -3240,41 +3801,41 @@
       <c r="M116" s="29"/>
       <c r="N116" s="29"/>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A117" s="12"/>
-      <c r="B117" s="6"/>
-      <c r="C117" s="26"/>
-      <c r="D117" s="29"/>
-      <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
-      <c r="G117" s="29"/>
-      <c r="H117" s="29"/>
-      <c r="I117" s="29"/>
-      <c r="J117" s="29"/>
-      <c r="K117" s="29"/>
-      <c r="L117" s="29"/>
-      <c r="M117" s="29"/>
-      <c r="N117" s="29"/>
+    <row r="117" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A117" s="11"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="27"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="30"/>
+      <c r="F117" s="30"/>
+      <c r="G117" s="30"/>
+      <c r="H117" s="30"/>
+      <c r="I117" s="30"/>
+      <c r="J117" s="30"/>
+      <c r="K117" s="30"/>
+      <c r="L117" s="30"/>
+      <c r="M117" s="30"/>
+      <c r="N117" s="30"/>
     </row>
     <row r="118" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A118" s="11"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="27"/>
-      <c r="D118" s="30"/>
-      <c r="E118" s="30"/>
-      <c r="F118" s="30"/>
-      <c r="G118" s="30"/>
-      <c r="H118" s="30"/>
-      <c r="I118" s="30"/>
-      <c r="J118" s="30"/>
-      <c r="K118" s="30"/>
-      <c r="L118" s="30"/>
-      <c r="M118" s="30"/>
-      <c r="N118" s="30"/>
-    </row>
-    <row r="119" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A119" s="13"/>
-      <c r="B119" s="15"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="15"/>
+      <c r="C118" s="26"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="29"/>
+      <c r="F118" s="29"/>
+      <c r="G118" s="29"/>
+      <c r="H118" s="29"/>
+      <c r="I118" s="29"/>
+      <c r="J118" s="29"/>
+      <c r="K118" s="29"/>
+      <c r="L118" s="29"/>
+      <c r="M118" s="29"/>
+      <c r="N118" s="29"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A119" s="10"/>
+      <c r="B119" s="6"/>
       <c r="C119" s="26"/>
       <c r="D119" s="29"/>
       <c r="E119" s="29"/>
@@ -3289,7 +3850,7 @@
       <c r="N119" s="29"/>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A120" s="10"/>
+      <c r="A120" s="12"/>
       <c r="B120" s="6"/>
       <c r="C120" s="26"/>
       <c r="D120" s="29"/>
@@ -3304,104 +3865,104 @@
       <c r="M120" s="29"/>
       <c r="N120" s="29"/>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A121" s="12"/>
-      <c r="B121" s="6"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="29"/>
-      <c r="E121" s="29"/>
-      <c r="F121" s="29"/>
-      <c r="G121" s="29"/>
-      <c r="H121" s="29"/>
-      <c r="I121" s="29"/>
-      <c r="J121" s="29"/>
-      <c r="K121" s="29"/>
-      <c r="L121" s="29"/>
-      <c r="M121" s="29"/>
-      <c r="N121" s="29"/>
+    <row r="121" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A121" s="11"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="30"/>
+      <c r="E121" s="30"/>
+      <c r="F121" s="30"/>
+      <c r="G121" s="30"/>
+      <c r="H121" s="30"/>
+      <c r="I121" s="30"/>
+      <c r="J121" s="30"/>
+      <c r="K121" s="30"/>
+      <c r="L121" s="30"/>
+      <c r="M121" s="30"/>
+      <c r="N121" s="30"/>
     </row>
     <row r="122" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A122" s="11"/>
-      <c r="B122" s="8"/>
-      <c r="C122" s="27"/>
-      <c r="D122" s="30"/>
-      <c r="E122" s="30"/>
-      <c r="F122" s="30"/>
-      <c r="G122" s="30"/>
-      <c r="H122" s="30"/>
-      <c r="I122" s="30"/>
-      <c r="J122" s="30"/>
-      <c r="K122" s="30"/>
-      <c r="L122" s="30"/>
-      <c r="M122" s="30"/>
-      <c r="N122" s="30"/>
-    </row>
-    <row r="123" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A123" s="13"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="26"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="29"/>
+      <c r="F122" s="29"/>
+      <c r="G122" s="29"/>
+      <c r="H122" s="29"/>
+      <c r="I122" s="29"/>
+      <c r="J122" s="29"/>
+      <c r="K122" s="29"/>
+      <c r="L122" s="29"/>
+      <c r="M122" s="29"/>
+      <c r="N122" s="29"/>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A123" s="10"/>
       <c r="B123" s="6"/>
-      <c r="C123" s="26"/>
-      <c r="D123" s="29"/>
-      <c r="E123" s="29"/>
-      <c r="F123" s="29"/>
-      <c r="G123" s="29"/>
-      <c r="H123" s="29"/>
-      <c r="I123" s="29"/>
-      <c r="J123" s="29"/>
-      <c r="K123" s="29"/>
-      <c r="L123" s="29"/>
-      <c r="M123" s="29"/>
-      <c r="N123" s="29"/>
+      <c r="C123" s="28"/>
+      <c r="D123" s="28"/>
+      <c r="E123" s="28"/>
+      <c r="F123" s="28"/>
+      <c r="G123" s="28"/>
+      <c r="H123" s="28"/>
+      <c r="I123" s="28"/>
+      <c r="J123" s="28"/>
+      <c r="K123" s="28"/>
+      <c r="L123" s="28"/>
+      <c r="M123" s="28"/>
+      <c r="N123" s="28"/>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A124" s="10"/>
+      <c r="A124" s="12"/>
       <c r="B124" s="6"/>
-      <c r="C124" s="28"/>
-      <c r="D124" s="28"/>
-      <c r="E124" s="28"/>
-      <c r="F124" s="28"/>
-      <c r="G124" s="28"/>
-      <c r="H124" s="28"/>
-      <c r="I124" s="28"/>
-      <c r="J124" s="28"/>
-      <c r="K124" s="28"/>
-      <c r="L124" s="28"/>
-      <c r="M124" s="28"/>
-      <c r="N124" s="28"/>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A125" s="12"/>
-      <c r="B125" s="6"/>
-      <c r="C125" s="26"/>
-      <c r="D125" s="29"/>
-      <c r="E125" s="29"/>
-      <c r="F125" s="29"/>
-      <c r="G125" s="29"/>
-      <c r="H125" s="29"/>
-      <c r="I125" s="29"/>
-      <c r="J125" s="29"/>
-      <c r="K125" s="29"/>
-      <c r="L125" s="29"/>
-      <c r="M125" s="29"/>
-      <c r="N125" s="29"/>
+      <c r="C124" s="26"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="29"/>
+      <c r="F124" s="29"/>
+      <c r="G124" s="29"/>
+      <c r="H124" s="29"/>
+      <c r="I124" s="29"/>
+      <c r="J124" s="29"/>
+      <c r="K124" s="29"/>
+      <c r="L124" s="29"/>
+      <c r="M124" s="29"/>
+      <c r="N124" s="29"/>
+    </row>
+    <row r="125" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+      <c r="A125" s="11"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="27"/>
+      <c r="D125" s="30"/>
+      <c r="E125" s="30"/>
+      <c r="F125" s="30"/>
+      <c r="G125" s="30"/>
+      <c r="H125" s="30"/>
+      <c r="I125" s="30"/>
+      <c r="J125" s="30"/>
+      <c r="K125" s="30"/>
+      <c r="L125" s="30"/>
+      <c r="M125" s="30"/>
+      <c r="N125" s="30"/>
     </row>
     <row r="126" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A126" s="11"/>
-      <c r="B126" s="8"/>
-      <c r="C126" s="27"/>
-      <c r="D126" s="30"/>
-      <c r="E126" s="30"/>
-      <c r="F126" s="30"/>
-      <c r="G126" s="30"/>
-      <c r="H126" s="30"/>
-      <c r="I126" s="30"/>
-      <c r="J126" s="30"/>
-      <c r="K126" s="30"/>
-      <c r="L126" s="30"/>
-      <c r="M126" s="30"/>
-      <c r="N126" s="30"/>
+      <c r="A126" s="22"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="26"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="29"/>
+      <c r="F126" s="29"/>
+      <c r="G126" s="29"/>
+      <c r="H126" s="29"/>
+      <c r="I126" s="29"/>
+      <c r="J126" s="29"/>
+      <c r="K126" s="29"/>
+      <c r="L126" s="29"/>
+      <c r="M126" s="29"/>
+      <c r="N126" s="29"/>
     </row>
     <row r="127" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A127" s="22"/>
+      <c r="A127" s="13"/>
       <c r="B127" s="6"/>
       <c r="C127" s="26"/>
       <c r="D127" s="29"/>
@@ -3464,22 +4025,6 @@
       <c r="M130" s="29"/>
       <c r="N130" s="29"/>
     </row>
-    <row r="131" spans="1:14" ht="15" x14ac:dyDescent="0.3">
-      <c r="A131" s="13"/>
-      <c r="B131" s="6"/>
-      <c r="C131" s="26"/>
-      <c r="D131" s="29"/>
-      <c r="E131" s="29"/>
-      <c r="F131" s="29"/>
-      <c r="G131" s="29"/>
-      <c r="H131" s="29"/>
-      <c r="I131" s="29"/>
-      <c r="J131" s="29"/>
-      <c r="K131" s="29"/>
-      <c r="L131" s="29"/>
-      <c r="M131" s="29"/>
-      <c r="N131" s="29"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
DSE_FH_ScAg_005: Updated the requierements and the planning document
</commit_message>
<xml_diff>
--- a/1) Requirements/SWRA_20190405.xlsx
+++ b/1) Requirements/SWRA_20190405.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="227">
   <si>
     <t>No.</t>
   </si>
@@ -765,9 +765,6 @@
     <t>RQ-SYS.031-4</t>
   </si>
   <si>
-    <t>Error en la comunicación con el display</t>
-  </si>
-  <si>
     <t>Cyclomatic Complexity Analysis</t>
   </si>
   <si>
@@ -865,6 +862,9 @@
   </si>
   <si>
     <t>Based on evidence.</t>
+  </si>
+  <si>
+    <t>Display communication error detectable</t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1543,8 +1543,8 @@
   <dimension ref="A1:N151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3531,17 +3531,39 @@
       <c r="C59" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="23"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="23"/>
-      <c r="N59" s="23"/>
+      <c r="D59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="J59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="K59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="L59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="M59" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="N59" s="77" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
@@ -5721,8 +5743,8 @@
       <c r="C121" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D121" s="77" t="s">
-        <v>16</v>
+      <c r="D121" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="E121" s="77" t="s">
         <v>16</v>
@@ -5765,8 +5787,8 @@
       <c r="C122" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D122" s="77" t="s">
-        <v>16</v>
+      <c r="D122" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="E122" s="77" t="s">
         <v>16</v>
@@ -5809,8 +5831,8 @@
       <c r="C123" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D123" s="77" t="s">
-        <v>16</v>
+      <c r="D123" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="E123" s="77" t="s">
         <v>16</v>
@@ -5853,8 +5875,8 @@
       <c r="C124" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D124" s="77" t="s">
-        <v>16</v>
+      <c r="D124" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="E124" s="77" t="s">
         <v>16</v>
@@ -5892,13 +5914,13 @@
         <v>192</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>193</v>
+        <v>226</v>
       </c>
       <c r="C125" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D125" s="77" t="s">
-        <v>16</v>
+      <c r="D125" s="67" t="s">
+        <v>37</v>
       </c>
       <c r="E125" s="77" t="s">
         <v>16</v>
@@ -5933,7 +5955,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" s="12"/>
-      <c r="B126" s="6"/>
+      <c r="B126" s="69"/>
       <c r="C126" s="21"/>
       <c r="D126" s="23"/>
       <c r="E126" s="23"/>
@@ -5950,7 +5972,7 @@
     <row r="127" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A127" s="11"/>
       <c r="B127" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C127" s="22"/>
       <c r="D127" s="24"/>
@@ -5986,7 +6008,7 @@
         <v>184</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C129" s="77" t="s">
         <v>16</v>
@@ -6044,7 +6066,7 @@
     <row r="131" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A131" s="11"/>
       <c r="B131" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C131" s="22"/>
       <c r="D131" s="24"/>
@@ -6077,10 +6099,10 @@
     </row>
     <row r="133" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A133" s="71" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C133" s="77" t="s">
         <v>16</v>
@@ -6121,10 +6143,10 @@
     </row>
     <row r="134" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B134" s="69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C134" s="77" t="s">
         <v>16</v>
@@ -6165,10 +6187,10 @@
     </row>
     <row r="135" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="73" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B135" s="69" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C135" s="77" t="s">
         <v>16</v>
@@ -6209,10 +6231,10 @@
     </row>
     <row r="136" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="73" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B136" s="69" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C136" s="77" t="s">
         <v>16</v>
@@ -6253,10 +6275,10 @@
     </row>
     <row r="137" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="73" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B137" s="69" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C137" s="77" t="s">
         <v>16</v>
@@ -6297,10 +6319,10 @@
     </row>
     <row r="138" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B138" s="69" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C138" s="77" t="s">
         <v>16</v>
@@ -6358,7 +6380,7 @@
     <row r="140" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A140" s="11"/>
       <c r="B140" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C140" s="22"/>
       <c r="D140" s="24"/>
@@ -6391,10 +6413,10 @@
     </row>
     <row r="142" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A142" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C142" s="77" t="s">
         <v>16</v>
@@ -6435,10 +6457,10 @@
     </row>
     <row r="143" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A143" s="71" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C143" s="77" t="s">
         <v>16</v>
@@ -6479,7 +6501,7 @@
     </row>
     <row r="144" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="74" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B144" s="69" t="s">
         <v>1</v>
@@ -6523,10 +6545,10 @@
     </row>
     <row r="145" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="B145" s="69" t="s">
         <v>216</v>
-      </c>
-      <c r="B145" s="69" t="s">
-        <v>217</v>
       </c>
       <c r="C145" s="77" t="s">
         <v>16</v>
@@ -6567,10 +6589,10 @@
     </row>
     <row r="146" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A146" s="71" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C146" s="77" t="s">
         <v>16</v>
@@ -6611,10 +6633,10 @@
     </row>
     <row r="147" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B147" s="69" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C147" s="77" t="s">
         <v>16</v>
@@ -6655,10 +6677,10 @@
     </row>
     <row r="148" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="74" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B148" s="72" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C148" s="77" t="s">
         <v>16</v>
@@ -6699,10 +6721,10 @@
     </row>
     <row r="149" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="74" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B149" s="69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C149" s="77" t="s">
         <v>16</v>
@@ -6743,10 +6765,10 @@
     </row>
     <row r="150" spans="1:14" s="68" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="74" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C150" s="77" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
DSE_FH_ScAg_003: Update the requirements according to the project release
</commit_message>
<xml_diff>
--- a/1) Requirements/SWRA_20190405.xlsx
+++ b/1) Requirements/SWRA_20190405.xlsx
@@ -871,7 +871,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -954,6 +954,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1035,7 +1044,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1261,6 +1270,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1532,7 +1544,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1543,8 +1555,8 @@
   <dimension ref="A1:N151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D111" sqref="D111:N111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5445,38 +5457,38 @@
       <c r="C111" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="F111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="H111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="J111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="K111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="L111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="M111" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="N111" s="77" t="s">
-        <v>16</v>
+      <c r="D111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="E111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="F111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="G111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="H111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="I111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="J111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="K111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="L111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="M111" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="N111" s="80" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
@@ -5721,38 +5733,38 @@
       <c r="C121" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="F121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="H121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="J121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="K121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="L121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="M121" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="N121" s="77" t="s">
-        <v>16</v>
+      <c r="D121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="E121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="F121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="G121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="H121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="I121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="J121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="K121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="L121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="M121" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="N121" s="67" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.3">
@@ -5765,38 +5777,38 @@
       <c r="C122" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="F122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="H122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="J122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="K122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="L122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="M122" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="N122" s="77" t="s">
-        <v>16</v>
+      <c r="D122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="E122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="F122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="G122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="H122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="I122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="J122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="K122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="L122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="M122" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="N122" s="67" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.3">
@@ -5809,38 +5821,38 @@
       <c r="C123" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="F123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="H123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="J123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="K123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="L123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="M123" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="N123" s="77" t="s">
-        <v>16</v>
+      <c r="D123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="E123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="F123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="G123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="H123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="I123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="J123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="K123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="L123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="M123" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="N123" s="67" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
@@ -5853,38 +5865,38 @@
       <c r="C124" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="F124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="H124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="J124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="K124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="L124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="M124" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="N124" s="77" t="s">
-        <v>16</v>
+      <c r="D124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="E124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="F124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="G124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="H124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="I124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="J124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="K124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="L124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="M124" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="N124" s="67" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.3">
@@ -5897,38 +5909,38 @@
       <c r="C125" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="F125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="H125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="I125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="J125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="K125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="L125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="M125" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="N125" s="77" t="s">
-        <v>16</v>
+      <c r="D125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="E125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="F125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="G125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="H125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="I125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="J125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="K125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="L125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="M125" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="N125" s="67" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>